<commit_message>
update to logreg analysis
</commit_message>
<xml_diff>
--- a/graphics/tables_export.xlsx
+++ b/graphics/tables_export.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicic\Documents\Programming\bachelor\bachelor\graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicic\Documents\bachelor\graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4EC43CA-1DBC-4D56-94B0-8EC4DDE1290B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC89FC5-F881-4D3A-97A4-69A4D9796122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20475" yWindow="1710" windowWidth="12750" windowHeight="17385" activeTab="1" xr2:uid="{ED008690-620C-47FF-95F4-46302A57DDE1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{ED008690-620C-47FF-95F4-46302A57DDE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="90">
   <si>
     <t xml:space="preserve">                 Generalized Linear Model Regression Results                  </t>
   </si>
@@ -241,6 +243,72 @@
   </si>
   <si>
     <t>weightedAverageShsOut</t>
+  </si>
+  <si>
+    <t>Dep. Variable:                      y   No. Observations:                  712</t>
+  </si>
+  <si>
+    <t>Link Function:                  Logit   Scale:                          1.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covariance Type:            nonrobust                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                       coef    std err          z      P&gt;|z|      [0.025      0.975]</t>
+  </si>
+  <si>
+    <t>----------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Fri, 16 May 2025</t>
+  </si>
+  <si>
+    <t>deferredIncomeTax</t>
+  </si>
+  <si>
+    <t>unhealthy</t>
+  </si>
+  <si>
+    <t>Model:                            GLM   Df Residuals:                      704</t>
+  </si>
+  <si>
+    <t>Model Family:                Binomial   Df Model:                            7</t>
+  </si>
+  <si>
+    <t>Method:                          IRLS   Log-Likelihood:                -393.69</t>
+  </si>
+  <si>
+    <t>Date:                Fri, 16 May 2025   Deviance:                       787.38</t>
+  </si>
+  <si>
+    <t>Time:                        15:44:14   Pearson chi2:                 5.13e+03</t>
+  </si>
+  <si>
+    <t>No. Iterations:                     9   Pseudo R-squ. (CS):             0.2411</t>
+  </si>
+  <si>
+    <t>cashAndCashEquivalents            4.716e-10   8.89e-11      5.306      0.000    2.97e-10    6.46e-10</t>
+  </si>
+  <si>
+    <t>taxPayables                      -2.068e-09   6.35e-10     -3.257      0.001   -3.31e-09   -8.23e-10</t>
+  </si>
+  <si>
+    <t>deferredTaxLiabilitiesNonCurrent  1.113e-09   3.66e-10      3.040      0.002    3.96e-10    1.83e-09</t>
+  </si>
+  <si>
+    <t>commonStock                      -3.686e-10   1.78e-10     -2.068      0.039   -7.18e-10   -1.93e-11</t>
+  </si>
+  <si>
+    <t>researchAndDevelopmentExpenses    -4.53e-09   8.64e-10     -5.242      0.000   -6.22e-09   -2.84e-09</t>
+  </si>
+  <si>
+    <t>sellingAndMarketingExpenses       -8.69e-10   2.15e-10     -4.045      0.000   -1.29e-09   -4.48e-10</t>
+  </si>
+  <si>
+    <t>incomeTaxExpense                  -2.02e-09   5.49e-10     -3.681      0.000    -3.1e-09   -9.45e-10</t>
+  </si>
+  <si>
+    <t>weightedAverageShsOut             3.615e-09   9.33e-10      3.877      0.000    1.79e-09    5.44e-09</t>
   </si>
 </sst>
 </file>
@@ -620,19 +688,19 @@
       <selection activeCell="E13" sqref="A13:E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -646,7 +714,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -660,7 +728,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -674,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -688,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -702,7 +770,7 @@
         <v>-331.43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -716,7 +784,7 @@
         <v>662.87</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -730,7 +798,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -744,7 +812,7 @@
         <v>0.3629</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -752,12 +820,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -777,7 +845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -800,7 +868,7 @@
         <v>1.85E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -823,7 +891,7 @@
         <v>4.8299999999999999E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -846,7 +914,7 @@
         <v>-2.4599999999999998E-10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -869,7 +937,7 @@
         <v>1.3399999999999999E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -892,7 +960,7 @@
         <v>3.5300000000000002E-10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -915,7 +983,7 @@
         <v>4.8200000000000003E-9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -938,7 +1006,7 @@
         <v>1.2300000000000001E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -961,7 +1029,7 @@
         <v>5.8299999999999995E-10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -984,7 +1052,7 @@
         <v>9.89E-10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1007,7 +1075,7 @@
         <v>-1.6499999999999999E-8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1030,7 +1098,7 @@
         <v>5.45E-9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1053,7 +1121,7 @@
         <v>3.1E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1076,7 +1144,7 @@
         <v>9.5399999999999997E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1099,7 +1167,7 @@
         <v>3.0499999999999998E-11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1122,7 +1190,7 @@
         <v>-3.7699999999999999E-10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1145,7 +1213,7 @@
         <v>-1.3699999999999999E-10</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1168,7 +1236,7 @@
         <v>1.27E-9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1191,7 +1259,7 @@
         <v>-9.89E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1214,7 +1282,7 @@
         <v>-3.2499999999999998E-11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1237,7 +1305,7 @@
         <v>-6.4199999999999995E-10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -1269,23 +1337,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD349B38-2F1F-4EB0-B813-B9009A907152}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1299,7 +1367,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1313,7 +1381,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1341,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1355,7 +1423,7 @@
         <v>-240.7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1437,7 @@
         <v>481.4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1383,7 +1451,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1397,7 +1465,7 @@
         <v>0.4758</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1405,12 +1473,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -1430,7 +1498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1453,7 +1521,7 @@
         <v>3.1E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1476,7 +1544,7 @@
         <v>4.7699999999999999E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1499,7 +1567,7 @@
         <v>9.5800000000000004E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1522,7 +1590,7 @@
         <v>5.6800000000000002E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1545,7 +1613,7 @@
         <v>-4.8999999999999996E-10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1568,7 +1636,7 @@
         <v>3.6399999999999998E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1591,7 +1659,7 @@
         <v>-8.2299999999999995E-10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1614,7 +1682,7 @@
         <v>4.9099999999999998E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1637,7 +1705,7 @@
         <v>-9.87E-9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1660,7 +1728,7 @@
         <v>2.18E-10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1683,7 +1751,7 @@
         <v>8.8599999999999996E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1706,7 +1774,7 @@
         <v>-7.5299999999999998E-10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1729,7 +1797,7 @@
         <v>1.4899999999999999E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1752,7 +1820,7 @@
         <v>-8.3600000000000001E-10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1775,7 +1843,7 @@
         <v>-3.58E-10</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1798,7 +1866,7 @@
         <v>-2.0799999999999998E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -1821,7 +1889,7 @@
         <v>-2.8499999999999999E-9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1844,7 +1912,7 @@
         <v>-2.5099999999999998E-9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1867,7 +1935,7 @@
         <v>6.8500000000000001E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1890,7 +1958,7 @@
         <v>-4.0199999999999998E-9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1913,7 +1981,7 @@
         <v>-4.1700000000000003E-9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -1936,7 +2004,7 @@
         <v>-4.7799999999999996E-9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1959,7 +2027,7 @@
         <v>1.0600000000000001E-8</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1967,4 +2035,655 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9021C3FA-7CCA-4DE3-82B6-3AE7EC4F07B0}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>-373.37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>746.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.59607638888888892</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>0.28320000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7.8899999999999996E-10</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.5199999999999999E-10</v>
+      </c>
+      <c r="D14">
+        <v>5.1820000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4.9099999999999996E-10</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.09E-9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.919E-10</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7.1900000000000005E-11</v>
+      </c>
+      <c r="D15">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="E15">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5.09E-11</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3.3299999999999999E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.951E-9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5.1999999999999996E-10</v>
+      </c>
+      <c r="D16">
+        <v>3.7509999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9.3099999999999999E-10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.9699999999999999E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7.5880000000000001E-10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.3900000000000002E-10</v>
+      </c>
+      <c r="D17">
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="E17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9.3800000000000002E-11</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.4200000000000001E-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4.1419999999999998E-10</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2.1E-10</v>
+      </c>
+      <c r="D18">
+        <v>1.9690000000000001</v>
+      </c>
+      <c r="E18">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.9600000000000001E-12</v>
+      </c>
+      <c r="G18" s="2">
+        <v>8.2700000000000004E-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-9.6309999999999991E-10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5.1E-10</v>
+      </c>
+      <c r="D19">
+        <v>-1.889</v>
+      </c>
+      <c r="E19">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1.9599999999999998E-9</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3.63E-11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-2.5720000000000001E-8</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.9200000000000002E-9</v>
+      </c>
+      <c r="D20">
+        <v>-4.3419999999999996</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-3.7300000000000003E-8</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-1.4100000000000001E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.6519999999999999E-9</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.15E-9</v>
+      </c>
+      <c r="D21">
+        <v>2.2989999999999999</v>
+      </c>
+      <c r="E21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3.9099999999999999E-10</v>
+      </c>
+      <c r="G21" s="2">
+        <v>4.9099999999999998E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4.4480000000000004E-9</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.3000000000000001E-9</v>
+      </c>
+      <c r="D22">
+        <v>3.427</v>
+      </c>
+      <c r="E22">
+        <v>1E-3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.9000000000000001E-9</v>
+      </c>
+      <c r="G22" s="2">
+        <v>6.9900000000000001E-9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="2">
+        <v>-1.1470000000000001E-9</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4.4300000000000002E-10</v>
+      </c>
+      <c r="D23">
+        <v>-2.5859999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23" s="2">
+        <v>-2.0200000000000001E-9</v>
+      </c>
+      <c r="G23" s="2">
+        <v>-2.7800000000000002E-10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2">
+        <v>-1.7380000000000001E-10</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4.5200000000000003E-11</v>
+      </c>
+      <c r="D24">
+        <v>-3.8460000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>-2.6200000000000003E-10</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-8.5300000000000005E-11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2">
+        <v>-4.318E-10</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.4000000000000001E-10</v>
+      </c>
+      <c r="D25">
+        <v>-3.0750000000000002</v>
+      </c>
+      <c r="E25">
+        <v>2E-3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>-7.0700000000000004E-10</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-1.57E-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2">
+        <v>-1.409E-9</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.0800000000000002E-10</v>
+      </c>
+      <c r="D26">
+        <v>-4.569</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>-2.0099999999999999E-9</v>
+      </c>
+      <c r="G26" s="2">
+        <v>-8.0500000000000001E-10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2">
+        <v>-3.1520000000000001E-10</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.0300000000000001E-10</v>
+      </c>
+      <c r="D27">
+        <v>-3.052</v>
+      </c>
+      <c r="E27">
+        <v>2E-3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-5.1799999999999997E-10</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-1.13E-10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2">
+        <v>-2.2670000000000001E-9</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5.4299999999999999E-10</v>
+      </c>
+      <c r="D28">
+        <v>-4.173</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-3.3299999999999999E-9</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-1.2E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D07639-C156-4941-815B-9B28F9A7B190}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to logred analysis
</commit_message>
<xml_diff>
--- a/graphics/tables_export.xlsx
+++ b/graphics/tables_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicic\Documents\bachelor\graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC89FC5-F881-4D3A-97A4-69A4D9796122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FBB00-B0BB-425D-9E6D-AF834636EB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{ED008690-620C-47FF-95F4-46302A57DDE1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
   <si>
     <t xml:space="preserve">                 Generalized Linear Model Regression Results                  </t>
   </si>
@@ -245,21 +245,6 @@
     <t>weightedAverageShsOut</t>
   </si>
   <si>
-    <t>Dep. Variable:                      y   No. Observations:                  712</t>
-  </si>
-  <si>
-    <t>Link Function:                  Logit   Scale:                          1.0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covariance Type:            nonrobust                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                       coef    std err          z      P&gt;|z|      [0.025      0.975]</t>
-  </si>
-  <si>
-    <t>----------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
     <t>Fri, 16 May 2025</t>
   </si>
   <si>
@@ -269,46 +254,10 @@
     <t>unhealthy</t>
   </si>
   <si>
-    <t>Model:                            GLM   Df Residuals:                      704</t>
-  </si>
-  <si>
-    <t>Model Family:                Binomial   Df Model:                            7</t>
-  </si>
-  <si>
-    <t>Method:                          IRLS   Log-Likelihood:                -393.69</t>
-  </si>
-  <si>
-    <t>Date:                Fri, 16 May 2025   Deviance:                       787.38</t>
-  </si>
-  <si>
-    <t>Time:                        15:44:14   Pearson chi2:                 5.13e+03</t>
-  </si>
-  <si>
-    <t>No. Iterations:                     9   Pseudo R-squ. (CS):             0.2411</t>
-  </si>
-  <si>
-    <t>cashAndCashEquivalents            4.716e-10   8.89e-11      5.306      0.000    2.97e-10    6.46e-10</t>
-  </si>
-  <si>
-    <t>taxPayables                      -2.068e-09   6.35e-10     -3.257      0.001   -3.31e-09   -8.23e-10</t>
-  </si>
-  <si>
-    <t>deferredTaxLiabilitiesNonCurrent  1.113e-09   3.66e-10      3.040      0.002    3.96e-10    1.83e-09</t>
-  </si>
-  <si>
-    <t>commonStock                      -3.686e-10   1.78e-10     -2.068      0.039   -7.18e-10   -1.93e-11</t>
-  </si>
-  <si>
-    <t>researchAndDevelopmentExpenses    -4.53e-09   8.64e-10     -5.242      0.000   -6.22e-09   -2.84e-09</t>
-  </si>
-  <si>
-    <t>sellingAndMarketingExpenses       -8.69e-10   2.15e-10     -4.045      0.000   -1.29e-09   -4.48e-10</t>
-  </si>
-  <si>
-    <t>incomeTaxExpense                  -2.02e-09   5.49e-10     -3.681      0.000    -3.1e-09   -9.45e-10</t>
-  </si>
-  <si>
-    <t>weightedAverageShsOut             3.615e-09   9.33e-10      3.877      0.000    1.79e-09    5.44e-09</t>
+    <t>===============================================================================================</t>
+  </si>
+  <si>
+    <t>taxPayables</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2011,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -2132,7 +2081,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -2319,7 +2268,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2">
         <v>-9.6309999999999991E-10</v>
@@ -2559,127 +2508,333 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D07639-C156-4941-815B-9B28F9A7B190}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>-402.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>805.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.71318287037037043</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>0.22109999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7.5699999999999997E-10</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.2199999999999999E-10</v>
+      </c>
+      <c r="D14">
+        <v>6.2080000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5.1799999999999997E-10</v>
+      </c>
+      <c r="G14" s="2">
+        <v>9.9600000000000008E-10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B15" s="2">
+        <v>-2.0139999999999999E-9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6.4099999999999996E-10</v>
+      </c>
+      <c r="D15">
+        <v>-3.1429999999999998</v>
+      </c>
+      <c r="E15">
+        <v>2E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-3.2700000000000001E-9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-7.5799999999999997E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2.9500000000000002E-10</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.28E-10</v>
+      </c>
+      <c r="D16">
+        <v>2.302</v>
+      </c>
+      <c r="E16">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>4.3899999999999998E-11</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5.4599999999999998E-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-1.8130000000000001E-8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.72E-9</v>
+      </c>
+      <c r="D17">
+        <v>-4.8730000000000002</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-2.5399999999999999E-8</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-1.0800000000000001E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-8.5390000000000002E-10</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.7699999999999999E-10</v>
+      </c>
+      <c r="D18">
+        <v>-2.2629999999999999</v>
+      </c>
+      <c r="E18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-1.5900000000000001E-9</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-1.1399999999999999E-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-1.2139999999999999E-9</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.5100000000000001E-10</v>
+      </c>
+      <c r="D19">
+        <v>-4.843</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1.6999999999999999E-9</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-7.2299999999999998E-10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-1.1100000000000001E-9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.4899999999999998E-10</v>
+      </c>
+      <c r="D20">
+        <v>-3.1789999999999998</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-1.79E-9</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-4.2599999999999998E-10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>